<commit_message>
Projeto de Regressao Logistica, Advertising
</commit_message>
<xml_diff>
--- a/Tabela Pokemon.xlsx
+++ b/Tabela Pokemon.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\rafael\Documents\Estudos\MeusProjetos\Ciência de Dados\Bases de Dados\Pokemon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\rafael\Documents\Estudos\Udemy\Python para Data Science e Machine Learning Completo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6600C4D6-5E88-49A2-A9F6-115E66D950DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7ADBFE-7010-4DA1-9F83-978D19D9F93C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E8C6A6BD-304C-45D0-9713-DC1493D71FD5}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="15375" windowHeight="7875" xr2:uid="{E8C6A6BD-304C-45D0-9713-DC1493D71FD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2856" uniqueCount="850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2927" uniqueCount="872">
   <si>
     <t>Nome</t>
   </si>
@@ -2575,6 +2575,72 @@
   </si>
   <si>
     <t>Rillaboom</t>
+  </si>
+  <si>
+    <t>Scorbunny</t>
+  </si>
+  <si>
+    <t>Raboot</t>
+  </si>
+  <si>
+    <t>Cinderace</t>
+  </si>
+  <si>
+    <t>Sobble</t>
+  </si>
+  <si>
+    <t>Drizzile</t>
+  </si>
+  <si>
+    <t>Inteleon</t>
+  </si>
+  <si>
+    <t>Skwovet</t>
+  </si>
+  <si>
+    <t>Greedent</t>
+  </si>
+  <si>
+    <t>Rookidee</t>
+  </si>
+  <si>
+    <t>Corvisquire</t>
+  </si>
+  <si>
+    <t>Corviknight</t>
+  </si>
+  <si>
+    <t>Blipbug</t>
+  </si>
+  <si>
+    <t>Dottler</t>
+  </si>
+  <si>
+    <t>Orbeetle</t>
+  </si>
+  <si>
+    <t>Nickit</t>
+  </si>
+  <si>
+    <t>Thievul</t>
+  </si>
+  <si>
+    <t>Gossifleur</t>
+  </si>
+  <si>
+    <t>Eldegoss</t>
+  </si>
+  <si>
+    <t>Wooloo</t>
+  </si>
+  <si>
+    <t>Dubwool</t>
+  </si>
+  <si>
+    <t>Chewtle</t>
+  </si>
+  <si>
+    <t>Drednaw</t>
   </si>
 </sst>
 </file>
@@ -2935,10 +3001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724C9910-21C1-4485-AA29-088EEC4C10A9}">
-  <dimension ref="A1:R813"/>
+  <dimension ref="A1:R835"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A808" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P813" sqref="P813"/>
+    <sheetView tabSelected="1" topLeftCell="A817" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A836" sqref="A836"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44232,7 +44298,7 @@
         <v>420</v>
       </c>
       <c r="Q727">
-        <f t="shared" ref="Q727:Q813" si="32">AVERAGE(J727:O727)</f>
+        <f t="shared" ref="Q727:Q835" si="32">AVERAGE(J727:O727)</f>
         <v>70</v>
       </c>
       <c r="R727" t="s">
@@ -49021,12 +49087,1237 @@
         <v>85</v>
       </c>
       <c r="P813">
-        <f t="shared" ref="P813" si="35">SUM(J813:O813)</f>
+        <f t="shared" ref="P813:P835" si="35">SUM(J813:O813)</f>
         <v>530</v>
       </c>
       <c r="Q813">
         <f t="shared" si="32"/>
         <v>88.333333333333329</v>
+      </c>
+      <c r="R813" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="814" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A814" t="s">
+        <v>850</v>
+      </c>
+      <c r="B814">
+        <v>813</v>
+      </c>
+      <c r="C814" t="s">
+        <v>23</v>
+      </c>
+      <c r="E814">
+        <v>0.3</v>
+      </c>
+      <c r="F814">
+        <v>4.5</v>
+      </c>
+      <c r="G814">
+        <v>45</v>
+      </c>
+      <c r="H814">
+        <v>87.5</v>
+      </c>
+      <c r="I814">
+        <v>12.5</v>
+      </c>
+      <c r="J814">
+        <v>50</v>
+      </c>
+      <c r="K814">
+        <v>71</v>
+      </c>
+      <c r="L814">
+        <v>40</v>
+      </c>
+      <c r="M814">
+        <v>40</v>
+      </c>
+      <c r="N814">
+        <v>40</v>
+      </c>
+      <c r="O814">
+        <v>69</v>
+      </c>
+      <c r="P814">
+        <f t="shared" si="35"/>
+        <v>310</v>
+      </c>
+      <c r="Q814">
+        <f t="shared" si="32"/>
+        <v>51.666666666666664</v>
+      </c>
+      <c r="R814" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="815" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A815" t="s">
+        <v>851</v>
+      </c>
+      <c r="B815">
+        <v>814</v>
+      </c>
+      <c r="C815" t="s">
+        <v>23</v>
+      </c>
+      <c r="E815">
+        <v>0.6</v>
+      </c>
+      <c r="F815">
+        <v>9</v>
+      </c>
+      <c r="G815">
+        <v>45</v>
+      </c>
+      <c r="H815">
+        <v>87.5</v>
+      </c>
+      <c r="I815">
+        <v>12.5</v>
+      </c>
+      <c r="J815">
+        <v>65</v>
+      </c>
+      <c r="K815">
+        <v>86</v>
+      </c>
+      <c r="L815">
+        <v>60</v>
+      </c>
+      <c r="M815">
+        <v>55</v>
+      </c>
+      <c r="N815">
+        <v>60</v>
+      </c>
+      <c r="O815">
+        <v>94</v>
+      </c>
+      <c r="P815">
+        <f t="shared" si="35"/>
+        <v>420</v>
+      </c>
+      <c r="Q815">
+        <f t="shared" si="32"/>
+        <v>70</v>
+      </c>
+      <c r="R815" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="816" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A816" t="s">
+        <v>852</v>
+      </c>
+      <c r="B816">
+        <v>815</v>
+      </c>
+      <c r="C816" t="s">
+        <v>23</v>
+      </c>
+      <c r="E816">
+        <v>1.4</v>
+      </c>
+      <c r="F816">
+        <v>33</v>
+      </c>
+      <c r="G816">
+        <v>45</v>
+      </c>
+      <c r="H816">
+        <v>87.5</v>
+      </c>
+      <c r="I816">
+        <v>12.5</v>
+      </c>
+      <c r="J816">
+        <v>80</v>
+      </c>
+      <c r="K816">
+        <v>116</v>
+      </c>
+      <c r="L816">
+        <v>75</v>
+      </c>
+      <c r="M816">
+        <v>65</v>
+      </c>
+      <c r="N816">
+        <v>75</v>
+      </c>
+      <c r="O816">
+        <v>119</v>
+      </c>
+      <c r="P816">
+        <f t="shared" si="35"/>
+        <v>530</v>
+      </c>
+      <c r="Q816">
+        <f t="shared" si="32"/>
+        <v>88.333333333333329</v>
+      </c>
+      <c r="R816" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="817" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A817" t="s">
+        <v>853</v>
+      </c>
+      <c r="B817">
+        <v>816</v>
+      </c>
+      <c r="C817" t="s">
+        <v>28</v>
+      </c>
+      <c r="E817">
+        <v>0.3</v>
+      </c>
+      <c r="F817">
+        <v>4</v>
+      </c>
+      <c r="G817">
+        <v>45</v>
+      </c>
+      <c r="H817">
+        <v>87.5</v>
+      </c>
+      <c r="I817">
+        <v>12.5</v>
+      </c>
+      <c r="J817">
+        <v>50</v>
+      </c>
+      <c r="K817">
+        <v>40</v>
+      </c>
+      <c r="L817">
+        <v>40</v>
+      </c>
+      <c r="M817">
+        <v>70</v>
+      </c>
+      <c r="N817">
+        <v>40</v>
+      </c>
+      <c r="O817">
+        <v>70</v>
+      </c>
+      <c r="P817">
+        <f t="shared" si="35"/>
+        <v>310</v>
+      </c>
+      <c r="Q817">
+        <f t="shared" si="32"/>
+        <v>51.666666666666664</v>
+      </c>
+      <c r="R817" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="818" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A818" t="s">
+        <v>854</v>
+      </c>
+      <c r="B818">
+        <v>817</v>
+      </c>
+      <c r="C818" t="s">
+        <v>28</v>
+      </c>
+      <c r="E818">
+        <v>0.7</v>
+      </c>
+      <c r="F818">
+        <v>11.5</v>
+      </c>
+      <c r="G818">
+        <v>45</v>
+      </c>
+      <c r="H818">
+        <v>87.5</v>
+      </c>
+      <c r="I818">
+        <v>12.5</v>
+      </c>
+      <c r="J818">
+        <v>65</v>
+      </c>
+      <c r="K818">
+        <v>60</v>
+      </c>
+      <c r="L818">
+        <v>55</v>
+      </c>
+      <c r="M818">
+        <v>95</v>
+      </c>
+      <c r="N818">
+        <v>55</v>
+      </c>
+      <c r="O818">
+        <v>90</v>
+      </c>
+      <c r="P818">
+        <f t="shared" si="35"/>
+        <v>420</v>
+      </c>
+      <c r="Q818">
+        <f t="shared" si="32"/>
+        <v>70</v>
+      </c>
+      <c r="R818" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="819" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A819" t="s">
+        <v>855</v>
+      </c>
+      <c r="B819">
+        <v>818</v>
+      </c>
+      <c r="C819" t="s">
+        <v>28</v>
+      </c>
+      <c r="E819">
+        <v>1.9</v>
+      </c>
+      <c r="F819">
+        <v>45.2</v>
+      </c>
+      <c r="G819">
+        <v>45</v>
+      </c>
+      <c r="H819">
+        <v>87.5</v>
+      </c>
+      <c r="I819">
+        <v>12.5</v>
+      </c>
+      <c r="J819">
+        <v>70</v>
+      </c>
+      <c r="K819">
+        <v>85</v>
+      </c>
+      <c r="L819">
+        <v>65</v>
+      </c>
+      <c r="M819">
+        <v>125</v>
+      </c>
+      <c r="N819">
+        <v>65</v>
+      </c>
+      <c r="O819">
+        <v>120</v>
+      </c>
+      <c r="P819">
+        <f t="shared" si="35"/>
+        <v>530</v>
+      </c>
+      <c r="Q819">
+        <f t="shared" si="32"/>
+        <v>88.333333333333329</v>
+      </c>
+      <c r="R819" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="820" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A820" t="s">
+        <v>856</v>
+      </c>
+      <c r="B820">
+        <v>819</v>
+      </c>
+      <c r="C820" t="s">
+        <v>172</v>
+      </c>
+      <c r="E820">
+        <v>0.3</v>
+      </c>
+      <c r="F820">
+        <v>2.5</v>
+      </c>
+      <c r="G820">
+        <v>255</v>
+      </c>
+      <c r="H820">
+        <v>50</v>
+      </c>
+      <c r="I820">
+        <v>50</v>
+      </c>
+      <c r="J820">
+        <v>70</v>
+      </c>
+      <c r="K820">
+        <v>55</v>
+      </c>
+      <c r="L820">
+        <v>55</v>
+      </c>
+      <c r="M820">
+        <v>35</v>
+      </c>
+      <c r="N820">
+        <v>35</v>
+      </c>
+      <c r="O820">
+        <v>25</v>
+      </c>
+      <c r="P820">
+        <f t="shared" si="35"/>
+        <v>275</v>
+      </c>
+      <c r="Q820">
+        <f t="shared" si="32"/>
+        <v>45.833333333333336</v>
+      </c>
+      <c r="R820" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="821" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A821" t="s">
+        <v>857</v>
+      </c>
+      <c r="B821">
+        <v>820</v>
+      </c>
+      <c r="C821" t="s">
+        <v>172</v>
+      </c>
+      <c r="E821">
+        <v>0.6</v>
+      </c>
+      <c r="F821">
+        <v>6</v>
+      </c>
+      <c r="G821">
+        <v>90</v>
+      </c>
+      <c r="H821">
+        <v>50</v>
+      </c>
+      <c r="I821">
+        <v>50</v>
+      </c>
+      <c r="J821">
+        <v>120</v>
+      </c>
+      <c r="K821">
+        <v>95</v>
+      </c>
+      <c r="L821">
+        <v>95</v>
+      </c>
+      <c r="M821">
+        <v>55</v>
+      </c>
+      <c r="N821">
+        <v>75</v>
+      </c>
+      <c r="O821">
+        <v>20</v>
+      </c>
+      <c r="P821">
+        <f t="shared" si="35"/>
+        <v>460</v>
+      </c>
+      <c r="Q821">
+        <f t="shared" si="32"/>
+        <v>76.666666666666671</v>
+      </c>
+      <c r="R821" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="822" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A822" t="s">
+        <v>858</v>
+      </c>
+      <c r="B822">
+        <v>821</v>
+      </c>
+      <c r="C822" t="s">
+        <v>24</v>
+      </c>
+      <c r="E822">
+        <v>0.2</v>
+      </c>
+      <c r="F822">
+        <v>1.8</v>
+      </c>
+      <c r="G822">
+        <v>255</v>
+      </c>
+      <c r="H822">
+        <v>50</v>
+      </c>
+      <c r="I822">
+        <v>50</v>
+      </c>
+      <c r="J822">
+        <v>38</v>
+      </c>
+      <c r="K822">
+        <v>47</v>
+      </c>
+      <c r="L822">
+        <v>35</v>
+      </c>
+      <c r="M822">
+        <v>33</v>
+      </c>
+      <c r="N822">
+        <v>35</v>
+      </c>
+      <c r="O822">
+        <v>57</v>
+      </c>
+      <c r="P822">
+        <f t="shared" si="35"/>
+        <v>245</v>
+      </c>
+      <c r="Q822">
+        <f t="shared" si="32"/>
+        <v>40.833333333333336</v>
+      </c>
+      <c r="R822" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="823" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A823" t="s">
+        <v>859</v>
+      </c>
+      <c r="B823">
+        <v>822</v>
+      </c>
+      <c r="C823" t="s">
+        <v>24</v>
+      </c>
+      <c r="E823">
+        <v>0.8</v>
+      </c>
+      <c r="F823">
+        <v>16</v>
+      </c>
+      <c r="G823">
+        <v>120</v>
+      </c>
+      <c r="H823">
+        <v>50</v>
+      </c>
+      <c r="I823">
+        <v>50</v>
+      </c>
+      <c r="J823">
+        <v>68</v>
+      </c>
+      <c r="K823">
+        <v>67</v>
+      </c>
+      <c r="L823">
+        <v>55</v>
+      </c>
+      <c r="M823">
+        <v>43</v>
+      </c>
+      <c r="N823">
+        <v>55</v>
+      </c>
+      <c r="O823">
+        <v>77</v>
+      </c>
+      <c r="P823">
+        <f t="shared" si="35"/>
+        <v>365</v>
+      </c>
+      <c r="Q823">
+        <f t="shared" si="32"/>
+        <v>60.833333333333336</v>
+      </c>
+      <c r="R823" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="824" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A824" t="s">
+        <v>860</v>
+      </c>
+      <c r="B824">
+        <v>823</v>
+      </c>
+      <c r="C824" t="s">
+        <v>24</v>
+      </c>
+      <c r="D824" t="s">
+        <v>179</v>
+      </c>
+      <c r="E824">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F824">
+        <v>75</v>
+      </c>
+      <c r="G824">
+        <v>45</v>
+      </c>
+      <c r="H824">
+        <v>50</v>
+      </c>
+      <c r="I824">
+        <v>50</v>
+      </c>
+      <c r="J824">
+        <v>98</v>
+      </c>
+      <c r="K824">
+        <v>87</v>
+      </c>
+      <c r="L824">
+        <v>105</v>
+      </c>
+      <c r="M824">
+        <v>53</v>
+      </c>
+      <c r="N824">
+        <v>85</v>
+      </c>
+      <c r="O824">
+        <v>67</v>
+      </c>
+      <c r="P824">
+        <f t="shared" si="35"/>
+        <v>495</v>
+      </c>
+      <c r="Q824">
+        <f t="shared" si="32"/>
+        <v>82.5</v>
+      </c>
+      <c r="R824" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="825" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A825" t="s">
+        <v>861</v>
+      </c>
+      <c r="B825">
+        <v>824</v>
+      </c>
+      <c r="C825" t="s">
+        <v>32</v>
+      </c>
+      <c r="E825">
+        <v>0.4</v>
+      </c>
+      <c r="F825">
+        <v>8</v>
+      </c>
+      <c r="G825">
+        <v>255</v>
+      </c>
+      <c r="H825">
+        <v>50</v>
+      </c>
+      <c r="I825">
+        <v>50</v>
+      </c>
+      <c r="J825">
+        <v>25</v>
+      </c>
+      <c r="K825">
+        <v>20</v>
+      </c>
+      <c r="L825">
+        <v>20</v>
+      </c>
+      <c r="M825">
+        <v>25</v>
+      </c>
+      <c r="N825">
+        <v>45</v>
+      </c>
+      <c r="O825">
+        <v>45</v>
+      </c>
+      <c r="P825">
+        <f t="shared" si="35"/>
+        <v>180</v>
+      </c>
+      <c r="Q825">
+        <f t="shared" si="32"/>
+        <v>30</v>
+      </c>
+      <c r="R825" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="826" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A826" t="s">
+        <v>862</v>
+      </c>
+      <c r="B826">
+        <v>825</v>
+      </c>
+      <c r="C826" t="s">
+        <v>32</v>
+      </c>
+      <c r="D826" t="s">
+        <v>177</v>
+      </c>
+      <c r="E826">
+        <v>0.4</v>
+      </c>
+      <c r="F826">
+        <v>19.5</v>
+      </c>
+      <c r="G826">
+        <v>120</v>
+      </c>
+      <c r="H826">
+        <v>50</v>
+      </c>
+      <c r="I826">
+        <v>50</v>
+      </c>
+      <c r="J826">
+        <v>50</v>
+      </c>
+      <c r="K826">
+        <v>35</v>
+      </c>
+      <c r="L826">
+        <v>80</v>
+      </c>
+      <c r="M826">
+        <v>50</v>
+      </c>
+      <c r="N826">
+        <v>90</v>
+      </c>
+      <c r="O826">
+        <v>30</v>
+      </c>
+      <c r="P826">
+        <f t="shared" si="35"/>
+        <v>335</v>
+      </c>
+      <c r="Q826">
+        <f t="shared" si="32"/>
+        <v>55.833333333333336</v>
+      </c>
+      <c r="R826" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="827" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A827" t="s">
+        <v>863</v>
+      </c>
+      <c r="B827">
+        <v>826</v>
+      </c>
+      <c r="C827" t="s">
+        <v>32</v>
+      </c>
+      <c r="D827" t="s">
+        <v>177</v>
+      </c>
+      <c r="E827">
+        <v>0.4</v>
+      </c>
+      <c r="F827">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="G827">
+        <v>45</v>
+      </c>
+      <c r="H827">
+        <v>50</v>
+      </c>
+      <c r="I827">
+        <v>50</v>
+      </c>
+      <c r="J827">
+        <v>60</v>
+      </c>
+      <c r="K827">
+        <v>45</v>
+      </c>
+      <c r="L827">
+        <v>110</v>
+      </c>
+      <c r="M827">
+        <v>80</v>
+      </c>
+      <c r="N827">
+        <v>120</v>
+      </c>
+      <c r="O827">
+        <v>90</v>
+      </c>
+      <c r="P827">
+        <f t="shared" si="35"/>
+        <v>505</v>
+      </c>
+      <c r="Q827">
+        <f t="shared" si="32"/>
+        <v>84.166666666666671</v>
+      </c>
+      <c r="R827" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="828" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A828" t="s">
+        <v>864</v>
+      </c>
+      <c r="B828">
+        <v>827</v>
+      </c>
+      <c r="C828" t="s">
+        <v>283</v>
+      </c>
+      <c r="E828">
+        <v>0.6</v>
+      </c>
+      <c r="F828">
+        <v>8.9</v>
+      </c>
+      <c r="G828">
+        <v>255</v>
+      </c>
+      <c r="H828">
+        <v>50</v>
+      </c>
+      <c r="I828">
+        <v>50</v>
+      </c>
+      <c r="J828">
+        <v>40</v>
+      </c>
+      <c r="K828">
+        <v>28</v>
+      </c>
+      <c r="L828">
+        <v>28</v>
+      </c>
+      <c r="M828">
+        <v>47</v>
+      </c>
+      <c r="N828">
+        <v>52</v>
+      </c>
+      <c r="O828">
+        <v>50</v>
+      </c>
+      <c r="P828">
+        <f t="shared" si="35"/>
+        <v>245</v>
+      </c>
+      <c r="Q828">
+        <f t="shared" si="32"/>
+        <v>40.833333333333336</v>
+      </c>
+      <c r="R828" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="829" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A829" t="s">
+        <v>865</v>
+      </c>
+      <c r="B829">
+        <v>828</v>
+      </c>
+      <c r="C829" t="s">
+        <v>283</v>
+      </c>
+      <c r="E829">
+        <v>1.2</v>
+      </c>
+      <c r="F829">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="G829">
+        <v>127</v>
+      </c>
+      <c r="H829">
+        <v>50</v>
+      </c>
+      <c r="I829">
+        <v>50</v>
+      </c>
+      <c r="J829">
+        <v>70</v>
+      </c>
+      <c r="K829">
+        <v>58</v>
+      </c>
+      <c r="L829">
+        <v>58</v>
+      </c>
+      <c r="M829">
+        <v>87</v>
+      </c>
+      <c r="N829">
+        <v>92</v>
+      </c>
+      <c r="O829">
+        <v>90</v>
+      </c>
+      <c r="P829">
+        <f t="shared" si="35"/>
+        <v>455</v>
+      </c>
+      <c r="Q829">
+        <f t="shared" si="32"/>
+        <v>75.833333333333329</v>
+      </c>
+      <c r="R829" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="830" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A830" t="s">
+        <v>866</v>
+      </c>
+      <c r="B830">
+        <v>829</v>
+      </c>
+      <c r="C830" t="s">
+        <v>13</v>
+      </c>
+      <c r="E830">
+        <v>0.4</v>
+      </c>
+      <c r="F830">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G830">
+        <v>190</v>
+      </c>
+      <c r="H830">
+        <v>50</v>
+      </c>
+      <c r="I830">
+        <v>50</v>
+      </c>
+      <c r="J830">
+        <v>40</v>
+      </c>
+      <c r="K830">
+        <v>40</v>
+      </c>
+      <c r="L830">
+        <v>60</v>
+      </c>
+      <c r="M830">
+        <v>40</v>
+      </c>
+      <c r="N830">
+        <v>60</v>
+      </c>
+      <c r="O830">
+        <v>10</v>
+      </c>
+      <c r="P830">
+        <f t="shared" si="35"/>
+        <v>250</v>
+      </c>
+      <c r="Q830">
+        <f t="shared" si="32"/>
+        <v>41.666666666666664</v>
+      </c>
+      <c r="R830" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="831" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A831" t="s">
+        <v>867</v>
+      </c>
+      <c r="B831">
+        <v>830</v>
+      </c>
+      <c r="C831" t="s">
+        <v>13</v>
+      </c>
+      <c r="E831">
+        <v>0.5</v>
+      </c>
+      <c r="F831">
+        <v>2.5</v>
+      </c>
+      <c r="G831">
+        <v>75</v>
+      </c>
+      <c r="H831">
+        <v>50</v>
+      </c>
+      <c r="I831">
+        <v>50</v>
+      </c>
+      <c r="J831">
+        <v>60</v>
+      </c>
+      <c r="K831">
+        <v>50</v>
+      </c>
+      <c r="L831">
+        <v>90</v>
+      </c>
+      <c r="M831">
+        <v>80</v>
+      </c>
+      <c r="N831">
+        <v>120</v>
+      </c>
+      <c r="O831">
+        <v>60</v>
+      </c>
+      <c r="P831">
+        <f t="shared" si="35"/>
+        <v>460</v>
+      </c>
+      <c r="Q831">
+        <f t="shared" si="32"/>
+        <v>76.666666666666671</v>
+      </c>
+      <c r="R831" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="832" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A832" t="s">
+        <v>868</v>
+      </c>
+      <c r="B832">
+        <v>831</v>
+      </c>
+      <c r="C832" t="s">
+        <v>172</v>
+      </c>
+      <c r="E832">
+        <v>0.6</v>
+      </c>
+      <c r="F832">
+        <v>6</v>
+      </c>
+      <c r="G832">
+        <v>255</v>
+      </c>
+      <c r="H832">
+        <v>50</v>
+      </c>
+      <c r="I832">
+        <v>50</v>
+      </c>
+      <c r="J832">
+        <v>42</v>
+      </c>
+      <c r="K832">
+        <v>40</v>
+      </c>
+      <c r="L832">
+        <v>55</v>
+      </c>
+      <c r="M832">
+        <v>40</v>
+      </c>
+      <c r="N832">
+        <v>45</v>
+      </c>
+      <c r="O832">
+        <v>48</v>
+      </c>
+      <c r="P832">
+        <f t="shared" si="35"/>
+        <v>270</v>
+      </c>
+      <c r="Q832">
+        <f t="shared" si="32"/>
+        <v>45</v>
+      </c>
+      <c r="R832" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="833" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A833" t="s">
+        <v>869</v>
+      </c>
+      <c r="B833">
+        <v>832</v>
+      </c>
+      <c r="C833" t="s">
+        <v>172</v>
+      </c>
+      <c r="E833">
+        <v>1.3</v>
+      </c>
+      <c r="F833">
+        <v>43</v>
+      </c>
+      <c r="G833">
+        <v>127</v>
+      </c>
+      <c r="H833">
+        <v>50</v>
+      </c>
+      <c r="I833">
+        <v>50</v>
+      </c>
+      <c r="J833">
+        <v>72</v>
+      </c>
+      <c r="K833">
+        <v>80</v>
+      </c>
+      <c r="L833">
+        <v>100</v>
+      </c>
+      <c r="M833">
+        <v>60</v>
+      </c>
+      <c r="N833">
+        <v>90</v>
+      </c>
+      <c r="O833">
+        <v>88</v>
+      </c>
+      <c r="P833">
+        <f t="shared" si="35"/>
+        <v>490</v>
+      </c>
+      <c r="Q833">
+        <f t="shared" si="32"/>
+        <v>81.666666666666671</v>
+      </c>
+      <c r="R833" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="834" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A834" t="s">
+        <v>870</v>
+      </c>
+      <c r="B834">
+        <v>833</v>
+      </c>
+      <c r="C834" t="s">
+        <v>28</v>
+      </c>
+      <c r="E834">
+        <v>0.3</v>
+      </c>
+      <c r="F834">
+        <v>8.5</v>
+      </c>
+      <c r="G834">
+        <v>255</v>
+      </c>
+      <c r="H834">
+        <v>50</v>
+      </c>
+      <c r="I834">
+        <v>50</v>
+      </c>
+      <c r="J834">
+        <v>50</v>
+      </c>
+      <c r="K834">
+        <v>64</v>
+      </c>
+      <c r="L834">
+        <v>50</v>
+      </c>
+      <c r="M834">
+        <v>38</v>
+      </c>
+      <c r="N834">
+        <v>38</v>
+      </c>
+      <c r="O834">
+        <v>44</v>
+      </c>
+      <c r="P834">
+        <f t="shared" si="35"/>
+        <v>284</v>
+      </c>
+      <c r="Q834">
+        <f t="shared" si="32"/>
+        <v>47.333333333333336</v>
+      </c>
+      <c r="R834" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="835" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A835" t="s">
+        <v>871</v>
+      </c>
+      <c r="B835">
+        <v>834</v>
+      </c>
+      <c r="C835" t="s">
+        <v>28</v>
+      </c>
+      <c r="D835" t="s">
+        <v>178</v>
+      </c>
+      <c r="E835">
+        <v>1</v>
+      </c>
+      <c r="F835">
+        <v>115.5</v>
+      </c>
+      <c r="G835">
+        <v>75</v>
+      </c>
+      <c r="H835">
+        <v>50</v>
+      </c>
+      <c r="I835">
+        <v>50</v>
+      </c>
+      <c r="J835">
+        <v>90</v>
+      </c>
+      <c r="K835">
+        <v>115</v>
+      </c>
+      <c r="L835">
+        <v>90</v>
+      </c>
+      <c r="M835">
+        <v>48</v>
+      </c>
+      <c r="N835">
+        <v>68</v>
+      </c>
+      <c r="O835">
+        <v>74</v>
+      </c>
+      <c r="P835">
+        <f t="shared" si="35"/>
+        <v>485</v>
+      </c>
+      <c r="Q835">
+        <f t="shared" si="32"/>
+        <v>80.833333333333329</v>
+      </c>
+      <c r="R835" t="s">
+        <v>438</v>
       </c>
     </row>
   </sheetData>

</xml_diff>